<commit_message>
Chagning all / to || in instructions and remove "
</commit_message>
<xml_diff>
--- a/database/COSC345_Recipes (1).xlsx
+++ b/database/COSC345_Recipes (1).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadia\Downloads\UNI-work\COSC345\Realm-of-Feasts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadia\Downloads\UNI-work\COSC345\Realm-of-Feasts\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBAFF85F-B94F-4779-8204-BAC7B91AE5D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B27A680-6F61-4242-A969-1AA988DEA456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{D48BFF6E-7DE3-47B5-ADE0-6EAA34E0C134}"/>
   </bookViews>
@@ -68,9 +68,6 @@
     <t>Simple instant ramen</t>
   </si>
   <si>
-    <t>1. Boil the water./2. Place the noodles in a ramen bowl. Pour boiling water over the noodles and cover. Set and start your timer for three minutes./3. After the first minute, quickly open, shake the noodles to separate, then arrange the ham, egg, and green onion over the noodles. Cover again and wait until the timer beeps.</t>
-  </si>
-  <si>
     <t>Easy</t>
   </si>
   <si>
@@ -98,9 +95,6 @@
     <t>2*thick slices*Bacon, 4*null*Eggs, 0*null*Sliced Bread, 0*null*Cheese, 0*null*Salt, 0*null*Pepper</t>
   </si>
   <si>
-    <t>1. Fry strips of bacon in a cast iron skillet over medium low heat. This keeps the bacon from burning while the fat renders out./ 2.Once the fat has rendered out, add cracked eggs to the pan. Cook until the eggs have a good crust on them. If the whites need to cook more, kill the heat to the pan and cover with a lid to steam the tops of the egg whites./3. Serve the eggs and bacon with some sliced bread and cheese and a good sprinkle of salt and pepper. Enjoy!</t>
-  </si>
-  <si>
     <t>Herring Pie or Fish Pie</t>
   </si>
   <si>
@@ -131,9 +125,6 @@
     <t>0*null*Rice, 0*null*Umeboshi (Pickled Plum), 0*null*Edamame, 0*null*Shishamo Fish (Smelt Fish), 1*fillet*Cod Fish, 0*null*Kombu (Seaweed), 2*tablespoons*Sake, 2*tablespoons*Sugar, 1*teaspoon*Salt, 0*null*Red Food Colouring</t>
   </si>
   <si>
-    <t>1. Cook Rice./2. Prepare Shishamo fish:Shishamo fish (or like fish) is usually sold frozen. Defrost and set frying pan to medium heat. And some oil and cook shishamo for about 5 minutes until crispy. Flip over and cook the other side for another 5 minutes. Place on a paper towel to soak the extra oil./3. Prepare the Sakura Denbu: Sakura Denbu is a type of "furikake", a condiment to put on top of rice.  It's salty-sweet and commonly pink to represent cherry blossoms. Boil water and add kombu and whole cod. The cod is cooked when you can break it into pieces easily. Drain the cod well. Use a paper towel to squeeze out the extra water from the fish. The dryer, the better is will look as flakes. On a plate, take out any extra bones. Prepare a pan or pot on medium-low heat. Add 2 Tbsp sake, 2 Tbsp sugar, 1 tsp salt to pan, then add the cod. Use chopsticks or other utensil that will break the cod into small flakes. Stir well until liquid evaporates. Lower the heat if the cod starts to over cook. Remove from heat once liquid evaporates. Add two drops of red food coloring and add a little bit of water (you can make the color light or darker to your choosing). Add the food coloring mixture to the cod.  Put under low heat if the flakes get mushy from the water.  Mix well until you get your desired pink color./4. Prepare the edamame: Boil frozen edamame for 6-10 minutes. Drain water in a colander and shuck the beans./5. Assemble all in the lunch box to look cute.</t>
-  </si>
-  <si>
     <t>Siberia Sponge Cake</t>
   </si>
   <si>
@@ -146,9 +137,6 @@
     <t>115*grams*Unsalted Butter, 115*mL*Milk, 7*null*Large Eggs (Room temp), 115*grams*Cake or AP Flour, 115*grams*White Sugar, 120*mL*Water, 10*grams*Gelatin or Agar Agar, 500*grams*Smooth Red Bean Paste</t>
   </si>
   <si>
-    <t>1. Preheat your oven to 150C. In a small saucepan add in your butter and milk and over medium heat, melt the butter, stirring occasionally. Remove from heat to slightly cool before using. Optional: You can also melt down 1 tbsp of honey with this mixture if you don't like eggy tasting cakes./2. Separate the whites and yolks of the eggs. Leave whites aside for meringue./3. Sieve the flour into a large mixing bowl. Add in your warm butter and milk mixture until well combined (it may look like dough, that's okay). Then in 3-4 additions, mix in your egg yolks until you have a thick batter. Optional: Add 1 tsp of vanilla extract with eggs if you don't like eggy tasting cakes./4. Whisk your egg whites on medium speed while adding your sugar in a slow, steady stream. Once all the sugar is added, continue whisking until you reach soft peaks (mixture will stay on your whisk, but the tip of the meringue droops)./5. Add your egg yolk mixture to the meringue and gently fold the two mixtures together until well combined and homogenous in colour./6. Line your baking tins with non-stick spray and baking paper, ensuring to leave overhang for easy removal. Wrap the base of the cake tins with aluminum foil (if they're loose bottom) to ensure water doesn't get into the cakes./7. Divide the batter between the two tins, and level out the surfaces. Place on your baking/roasting tray and fill with 2cm worth of hot water./8. Transfer into oven and bake at 150c for 1 hour and the cakes are golden brown./9. Remove cakes from the oven and allow to cool for 10 minutes before removing from tins to fully cool./10. In a medium saucepan, bring the water to a boil and stir in gelatin or agar until fully dissolved. Mix in red bean paste until dissolved, thick and glossy. Set aside to cool./11. Line one baking tin with plastic wrap on all sides, ensuring to leave overhang for easy removal. Place 1 cake, golden side down into the tin. Then add the red bean paste, spreading it out in an even layer. Then, top with remaining cake, golden side up. Refrigerate for 4 hours or until red bean filling is set./12. When the filling is set, remove the cake from the tray, trim the edges of the cake to show off the well-defined layers. Cut the cake into 8 equal triangles and enjoy!</t>
-  </si>
-  <si>
     <t>Spaghetti Bolognese</t>
   </si>
   <si>
@@ -206,9 +194,6 @@
     <t>High tea cake with lemon swiss meringue butter cream</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Preheat oven to 160C fan forced./2. In the bowl of a stand mixer, add the oil, egg yolks, water and vanilla extract. Beat over medium-high speed for 30 seconds or until emulsified./3. Sift in the flour, baking powder, salt and add 118 grams of white sugar. Beat over medium speed until just combined and no lumps remain, about 1-2 minutes./4. In a separate bowl, whisk the egg whites (NOT the 90g Egg whites) until foamy. Add the cream of tartar and continue whisking until soft peaks are achieved./5. Then slowly add in 50 grams of white sugar and continue to whisk until the meringue reaches stiff peaks./6. Add 1/3 of the meringue into the egg-yolk batter and whisk to combine. Add another 1/3 of the meringue and gently fold together until no white streaks remain. Repeat folding process with the final 1/3 of the meringue./7. Line the base of a loose bottomed 8-inch cake pan with oil and baking paper. Gently pour the mixture into the pan, smooth the surface with a spatula and tap against the counter a few times to level the cake./8. Transfer into the oven and bake for 45-50 minutes, or until a skewer can be inserted into the centre of the cake and when removed, it comes out clean. Allow to cool completely in the pan./9. Over a pot of simmering water, place over a stand mixer/heatproof bowl ensuring the water is not touching the bowl./10. Add 100g sugar, egg whites, lemon juice and lemon zest into the bowl and whisk until sugar is completely dissolved./11. Remove the bowl and attach to your stand mixer. Whisk meringue over high speed until the meringue and bowl are cool to the touch./12. Reduce speed to medium-low and add in the softened butter 1tbsp at a time, ensuring each addition of butter is fully incorporated before adding more. Scrape down the bowl as necessary./13. After adding all the butter, beat for an additional 2 minutes./14. To ice the cake, apply a thin layer of buttercream all over the cake and refrigerate for 10-15 minutes or until the buttercream is firm to the touch. Once firm, remove from the fridge and apply a final layer of buttercream onto the cake. </t>
-  </si>
-  <si>
     <t>Japanese Butter Cookies and Jam Cookies</t>
   </si>
   <si>
@@ -242,9 +227,6 @@
     <t xml:space="preserve">0*null*Cooked Rice, 0*null*Miso Soup, 0*null*Ham, 0*null*Natto, 2*null*Eggs, 1.5*tablespoon*Soy Sauce, 3*teaspoons*Sugar, 1*head*Spinach, 1*pinch*Salt, 0*null*Sesame, 10*grams*Dried Bonito, 1*tablespoon*Sweet Sake (Mirin), 1*piece*Umeboshi, 0.5*piece*Mentaiko </t>
   </si>
   <si>
-    <t>1. Cut the spinach into 5 cm width./2. Put oil in a frying pan and fry the spinach./3. Season with salt, add sesame seeds and mix./4. Crack 2 eggs, add soy sauce and sugar, and mix./5. Spread oil on a frying pan and spread 1/3 of the egg mixture. Fold the egg several times./6. Spread oil again, add half of the remaining egg mixture and spread. Fold the eggs together with (5)./7. Spread the oil again, add the rest of the egg mixture, spread it out, and fold the egg of (6)./8. Add the seasoning for the bonito flakes to the frying pan, mix, and bring to a boil./9. Add katsuobushi and mix./10. Lightly heat the mentaiko./11. Cut the mentaiko in half and the egg into bite-sized pieces./12. Arrange in a bento box with rice, ham, and natto./13. Serve with miso soup on the side</t>
-  </si>
-  <si>
     <t>Nimono Stew</t>
   </si>
   <si>
@@ -281,9 +263,6 @@
     <t>1*null*Pasteurised Egg, 1*bowl*Rice, 0*null*Soy Sauce</t>
   </si>
   <si>
-    <t>1. Prepare a bowl of rice./2. Crack the egg on top of the rice./3. Drizzle with soy sauce to taste./4. Mix well.</t>
-  </si>
-  <si>
     <t>Salmon with Cream Sauce</t>
   </si>
   <si>
@@ -293,9 +272,6 @@
     <t>3*fillets*Salmon, 1*packet*Baby Carrots, 1*cup*Water, 6*tablespoons*Butter, 2*tablespoons*Brown Sugar, 2*tablespoons*Lemon Juice, 0*null*Salt, 0*null*Black Pepper, 2*tablespoons*All Purpose Flour, 1*cup*Milk</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Remove salmon skin and season the salmon with salt and pepper./2. Add 2 tbsp of butter into a saucepan and heat on medium-low. Fry the salmon until both sides turn golden brown./3. Melt 2 tbsp of butter in a saucepan over medium heat. Add chopped garlic and shallots. Stir well until the garlic turns light brown./4. Lower the heat to medium-low and add flour. Mix well until the mixture thickens./5. Add milk while stirring. Mix until the mixture thickens again./6. Add baby carrots and 1 cup of water until it boils. Poke the carrots with a fork to check if it is soft enough./7. Drain the baby carrots and add 2 tbsp of butter. Add salt and pepper as seasoning./8. Add 2 tbsp of brown sugar. Mix well until the mixture thickens./9. Transfer the salmon onto a plate and pour the cream sauce over it. Place the glazed carrots on the side of the plate. </t>
-  </si>
-  <si>
     <t>Cream Stew</t>
   </si>
   <si>
@@ -314,42 +290,6 @@
     <t>Kiki's Delivery Service</t>
   </si>
   <si>
-    <t>1. Cut up the potatoes and put them in a pot of boiling water.  Boil for about 5 minutes, then add in two eggs and boil for 5 more minutes.  Take out the eggs, and strain the potatoes.  Then mash the potatoes in a bowl with 2/3 cup of milk./2.Add the mashed potatoes to the bottom of your casserole dish, saving about 1 potato worth of mash in the bowl./3. Slice all of the vegetables and the hardboiled eggs and saute them in a pan with some oil or butter and the bay leaves./4. Add in the rest of the milk, the mashed potato that you saved, mustard, salt and pepper.  Cook everything on medium heat stirring occasionally, until the milk reaches a thick consistency, then add it into the casserole pan.  Remember to remove the bay leaves./5. Cut the fish fillets into 3 inch wide chunks, and then add it into the casserole pan./6. Unroll the pie crust and put it on top. You can cut it into strips, and cut out a fish if you want to make it like the one in Kiki's Delivery Service. Once you finish covering the casserole pan with the pie crust, beat an egg and brush it on top of the pie crust./7. Bake in a 350 degree oven for about 20-30 minutes, or until the crust is to your liking.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Add the flour, sugar, yeast and salt into a bowl, ensuring that the salt and yeast aren't touching. Mix thoroughly to combine. Add the water and oil, then mix with a wooden spoon until it comes together as a rough dough./ 2. Turn the dough out onto a lightly floured work surface and knead by hand (or in a stand mixer) for 10 minutes or until soft, smooth and elastic./3. Lightly coat a bowl in oil and transfer in your dough. Toss the dough in the bowl to ensure it's fully coated in oil. Cover and allow to proof until doubled in size (about an hour)./ 4. Uncover the dough and knock out the air. Flatten the dough into a large disc and make a well in the centre. Add the baking powder into the well and gather the edges of the dough towards the centre to enclose the baking powder./5. Knead the dough for a few minutes or until the baking powder is well distributed into the dough. Flatten the dough and then divide the dough into 6 to 12 even pieces, cover any dough that isn't being used to prevent it from drying out./6. Pat out your portioned dough into a disc and spread over a layer of red bean paste. Cup the dough in both hands and gently rotate the dough until the edges are nearly touching. Gather the edges together and twist to seal. Invert the dough so that the seam is on your work surface. Gently roll it around to help tighten that seal. Cover and rest the buns for another 20 minutes. Line your steamers and bring water to a boil in a saucepan during that time./7. Transfer the buns into a steamer lined with some baking paper, making sure to leave space between each bun as they will expand. Cover with a lid, place the steamer onto your saucepan, reduce heat to a simmer and allow to steam, undisturbed for 12 to 15 minutes (20 minutes if you want to make a massive one). Remove from heat and allow to rest for 5 minutes before opening the lid. Eat them while they're still warm! </t>
-  </si>
-  <si>
-    <t>1. You'll actually want to start with your frosting, since it needs extra time to chill (in fact, you can make the frosting a day ahead of time if you want). First, place your chocolate chips in a large bowl and set aside./2. Cook the whipping cream and butter in a saucepan over medium heat until just boiling, stirring frequently. Pour the cream mix over the chocolate and whisk briskly until completely smooth./3. Place some plastic wrap over the bowl and put it in the fridge to chill. After 1 hour, stir the mix thoroughly. Replace the cover and put the mix back in the fridge for another hour or until it reaches spreading consistency./4. While you're waiting for the frosting to chill, you can bake your cake! Preheat your oven to 350 degrees. Thoroughly spray a 9-inch round cake pan with cooking spray or grease it with butter and flour. This cake likes to stick, so be sure to thoroughly coat every nook and cranny./5. Dump the sugar, flour, cocoa, baking soda, baking powder, and salt into a large bowl. Whisk it all up!/6. Whisk in the egg, buttermilk, coffee, oil and vanilla. Beat the mix briskly for 2 minutes./7. Pour the batter into your pan and bake for 25-30 minutes or until a toothpick inserted in the center comes out clean./8. When fully baked, set the cake pan on a wire rack to cool for 10 minutes. Then flip the cake out of the pan and allow it to cool completely on the rack./9. When the cake is cool, spread on a layer of chocolate frosting. Let it set for 5-10 minutes./10. Use a toothpick to draw out where you'll put the decorative icing. This makes it easier to replicate the look of the cake in the movie. If you make a mistake, just use an icing knife or butter knife to smooth it out./11. Pipe your decorative icing over the toothpick drawing and allow it to set for another 5-10 minutes.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Gather all the ingredients. I follow a rice-to-water ratio of 1 to 5 for a thicker consistency in this recipe; to adjust for a runnier consistency, please see the Notes at the end of the recipe card./2. Rinse 0.25 cup uncooked Japanese short-grain white rice in water, then drain. Repeat until the water runs clear. Drain into a colander and shake off the excess water./3. Add the well-drained rice and 250 ml water to a heavy-bottomed pot or a donabe earthenware pot, as I have here. If cooking in a donabe, use a towel to wipe off any excess water on the bottom of the pot (or else it may crack under heat). Tip: Select a cooking pot with plenty of room for the rice and water to cook without boiling over./4. Soak the rice for at least 30 minutes./5. Cover the pot and bring to a boil over high heat./5. Once boiling, lower the heat to the stove's lowest setting (make sure to use the right size of stove burner for your pot size). Open the lid and gently mix with a spoon, making sure the rice does not stick to the bottom of the pot./6. Then, cover with the lid and gently simmer the rice for 30 minutes. During this time, I do not open the lid or mix the rice. Tip: With a good size pot and the lowest heat on the stove, the water should not boil over. If you cook with more water or your pot is smaller than mine, you may want to leave the lid slightly ajar so the water doesn't boil over. Tip: If you are worried, you can take a quick peek to make sure there's enough water so the rice doesn't burn on the bottom of the pot. If necessary, you can stir the rice or add a bit of hot water. Otherwise, don't stir the rice because that may break the rice grains./7. After 30 minutes, turn off the heat and let it steam with the lid on for 10 minutes. The rice porridge should be soft and thick. If you want to add a beaten egg or salt, this is the time to mix it in. I keep this recipe plain and simple. Serve in individual rice bowls and garnish with toppings of your choice./8. You can keep the leftovers in an airtight container and keep them for 2 days in the refrigerator or for up to a month in the freezer. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Chop the carrots, broccoli, cauliflower, and potatoes into small pieces./2. Slice the leek into thin slices./3. Mince the garlic./4. Heat olive oil on medium heat and cook the sliced leeks till it has softened./5. Add about 5 cups of water and 1 tsp of salt./6. When the water has reached a boil, add all of the chopped vegetables. Make sure that the vegetables are fully submerged in water./7. Boil for less than 5 minutes. Pierce with a fork to see if the vegetables are soft enough./8. Remove the vegetables from the pot and set it aside. /9. With the remaining water left in the pot, add flour and milk. Whisk until it reaches a thick consistency./10. Boil the mixture while whisking. Add the boiled vegetables and season it with salt and pepper./11. Transfer it to a bowl and garnish with parsley. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.Heat 2 tbsp oil in pan, add mushroom and saute till fragrant./2. Add in bamboo shoots and pork fillet. Fry till meat turn white./3. Add in seasoning and fried shallots and mix evenly. Remove from heat and set aside./4. Combine flour with water in a small mixing bowl, stir till well dissolved./5. Bring a pot of water to a simmer. Place the bowl of flour batter over the pot. Stirring constantly and cook till batter turns thick./6. Grease 4 small bowls with corn oil. Scoop some cooked batter into each bowl. Lightly grease your fingers and press out the dough to cover the base of the bowl. Fill in meat filling. Top with another layer of cooked dough covering the fillings completely. Using greased fingers to smoothen out the edge and surface. /7. Steam the meatballs over preheated steamer over high heat for 10 minutes. Cool down for 10 minutes./8. Heat some oil in pan, remove the meatballs from the bowl and pan fry them till lightly brown on both sides. Drain well and serve with sauce immediately./9. Optional sauce: mix and simmer 2 tablespoons sweet chilli sauce, 1 tablespoon miso paste, 4 tablespoon Hai Shan sauce, 1 tablespoon sugar, 100mL water. Add in corn starch after simmering to thicken. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. In a large bowl, beat the butter until light and creamy./2. Add the sugar and beat together until well combined./3. Add the vanilla and salt, continue to beat while adding the beaten egg in 3 to 4 additions./4. Add the flour and knead together until a cohesive dough is formed./5. Reserve half the dough to one side, adding the cocoa powder to the other half. Knead until well combined./6. Place each dough onto a sheet of baking paper. Pat into a flat rectangle, top with another sheet of baking paper and roll until 5mm in thickness. Refrigerate for 1 hour or until firm.Preheat oven to 160C fan forced./7. Cut the vanilla cookies into squares, then score horizontal and two vertical lines perpendicular to the edges of the cookies. Transfer to a lined baking tray./8. Cut the chocolate cookies using a 48mm fluted cookie cutter. Transfer to a lined baking tray, then cut out the centre of each cookie with a small round cutter/piping tip./9. Bake both sheets of cookies for 18-20 minutes. Remove chocolate cookies after 12 minutes, add in 0.5 tsp of crushed candy to each cookie centre, then continue to bake for remaining time./10. Allow to cool on the tray for 10 minutes before transferring to a wire rack. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Cut the carrots evenly: put your peeled carrot on the board, and cut at even intervals while giving a quarter-turn to the carrot each time. Or alternatively, slice carrots regularly and use a cookie cutter to create flower shaped carrots./2. Cut and prep the potatoes into fairly even pieces. Optionally, you can shave the edges of each piece to round them off. This cutting method is called mentori. Put the cut up potato in a bowl of water, and then drain to rinse off the surface starch/3. Cut the shiitake mushtooms: tightly squeeze out the rehydrated dried shiitake mushrooms, saving the soaking liquid. Cut off the stem, which is usually too chewy even after rehydrating. Cut each cap in half - but instead of just going straight up and down, make a slanted 45 degree cut./4. Cut the onion into 1/8th wedges./5. Heat up your pan with the teaspoon of oil.  Put the onions in first and stir around for 2-3 minutes until the edges start turning a bit translucent./5. Add the potatoes and carrots and continue stirring for a minute. This short sauteing step helps to bring out the sweetness of the vegetables. Add the mushrooms and stir a bit more./6. Add the dashi stock (or combined dashi + mushroom soaking liquid). There should be enough to just about come to the top level of all the vegetables in the pot./7. Bring it up to a boil and lower the heat to a simmer. Some scum will rise to the top, which should be removed so that the final dish will have a clean taste and appearance. Try to take off just the scum and leave the liquid. /8. Add the flavoring ingredients in this order: sugar, mirin, sake, and then finally the soy sauce./9. Let simmer on its own. In the meantime, blanch the peas in boiling water for a minute or two./10. Arrange the vegetables attractively in a bowl, pouring a little of the cooking liquid over it to add shine and flavor. Garnish with the snow peas or other green garnish of your choice to make it "pop". </t>
-  </si>
-  <si>
-    <t>1. In a medium bowl, whisk the salt into the flour. In a large mixing bowl on med-high speed, cream together the butter &amp; sugar until light &amp; fluffy. Mix in the egg &amp; flavoring until fully combined. Turn the speed to low &amp; gradually add in the flour &amp; beat until a smooth dough is formed. Lay out a large sheet of plastic wrap &amp; plop the cookie dough into the center. Wrap the dough &amp; shape it into a log about 1 1/2" in diameter. Wrap it again is foil &amp; then place it in the fridge for a couple hours or overnight./2. Line 2 large trays with parchment. Remove the dough from the fridge &amp; cut it into even slices between 1/4" -1/2" wide (this will give you uniform cookies). Roll 1 slice at a time in the palms of your hands to make dough balls &amp; place them on the trays about 2" apart. Press your thumb into the center of each ball to make a decent indentation, being careful not to go all the way through to the tray below (also, having short thumb nails is best). If the sides crack, simply press them back together./3. If you're using fruit preserves for the center, spoon a small amount into each thumbprint. Do not mound up the preserves, just let it be a flat little pool. If you're using candied cherries, simply cut them in half &amp; nestle one half-round side up-into each thumbprint. If using maraschino cherries, do the same thing after you've drained &amp; patted/gently squeezed them dry./4. Chill the cookie trays in the fridge while your oven preheats to 350degreesF. Bake 1 tray at a time on the middle rack for about 12 minutes, or until the cookie bottoms are just beginning to golden. Remove from the oven &amp; gently transfer the cookies to a cooling rack. If you'd like to sprinkle sugar over the cookies (gives them a more Christmas-y vibe), place the cooling rack over the empty baking tray &amp; dust the cookies with sifted powdered sugar, &amp; then let cool. To store, place in an airtight container with wax paper.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. In a large measuring cup or bowl, combine 3.3 cups dashi (Japanese soup stock), 2 Tbsp mirin, 2 Tbsp soy sauce, and 1 tsp Diamond Crystal kosher salt./2. Mix it all together until the salt is completely dissolved. Then, divide the soup broth into the individual donabe clay pots. Set aside./3. Cut 1 inch kamaboko (fish cake) into 4 thin slices about 0.25 inch thick. Cut 1 piece aburaage (deep-fried tofu pouch) into 4 rectangular pieces./4. Cut off and discard the stems of 2 shiitake mushrooms./5. Slice 1 Tokyo negi (naga negi; long green onion) diagonally into 0.5-inch (1.3-cm) pieces./6. Cut 2 stalks komatsuna or other green vegetable into 2-inch (5-cm) pieces. Keep the stem and leafy parts separate because we will add them to the broth at different times./7. To cook 2 servings udon noodles, bring a large pot of water to a boil. Once boiling, cook the frozen udon for 1 minute until heated through and drain well. If you use dried noodles, cook them according to the package instructions./8. Divide and add the udon noodles into the individual pots. Then, top the noodles with equal portions of the kamaboko fish cake, aburaage, shiitake mushroom, Tokyo negi, and green vegetable stems. (Set aside the eggs, leafy greens, and shrimp tempura for later.)/9. Transfer the pots to individual burners on the stovetop. Cover with the lids and bring the soup to a boil over medium heat. Once boiling, reduce the heat to a simmer and cook for 2-3 minutes./10. Uncover the pot. With 2 large eggs (50 g each w/o shell), crack one egg in the center of each pot on top of the ingredients. Cover to cook until the egg is done to your liking./11. Once the egg is done, add both the leafy greens and the cooked 4 shrimp tempura on top./12. Bring the donabe to the table. Sprinkle with shichimi togarashi (Japanese seven spice) and top with yuzu zest, if you'd like. </t>
-  </si>
-  <si>
-    <t>1. Start by slicing your nori sheets in half lengthwise. My sheets were 2.5" x 3.5", so in the end I had 12 strips that were 1.25" wide. Mix the mayonnaise into your salmon until well coated. Set the salmon mix and nori aside./2. Put the cookie cutter on a flat surface. Place an 8"x8" sheet of plastic wrap over the cookie cutter and push some of it it down inside so that the inside of the cookie cutter is completely lined with plastic wrap. Scoop approximately 2 tbsp of rice into the bottom of the cutter and press it flat with a plastic spoon or small rubber spatula (the rice won't stick to the tools as much as it sticks to fingers!). When flattening the rice, push it around so that it reaches right up to the corners of the cutter (add more rice if needed to make sure the bottom is completely coated). Place 1 tsp salmon filling into the middle of the rice, spreading it around just a little, so there will be a little salmon in each bite of rice when you're finished./3. Place a couple more tablespoons of rice on top and flatten out as before. Add a little extra rice if you need more to cover up the salmon. Wrap the plastic tightly over the exposed end of the onigiri and pop it out of the cookie cutter. Firmly wrap any loose ends around the outside of the onigiri. Set aside. /4. Repeat with remaining rice and salmon until you run out of ingredients (for me, this made 12 rice balls)./5. Let the onigiri set for 5-10 minutes. If planning to eat them later, place them on a baking sheet and chill until ready to serve (you can reheat them in the microwave inside the plastic wrap for no more than 20-25 seconds - if they get too hot, they can fall apart). /6. When ready to serve, remove the plastic wrap and press a nori strip around the bottom of each onigiri. The rice should still be sticky enough that the nori adheres with no problems.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Remove the scales on both sides of the fish by sliding the tip of the knife from the tail end towards the head./2. Place the knife where the tail begins, facing the blade to the head. Move the knife at a very low angle towards the head and trim the bony scales (scutes) along the lateral line, which ends close to half-way./3. Remove the head by cutting at a slight angle behind the gill and the front fin./4. Using a finger or a narrow knife, remove the guts from the opening, without breaking the thin flesh around the belly./5. Rinse the fish and clean the cavity in the belly. Pat dry, including inside the cavity. /6. Starting from the head of the fish, make a shallow incision on the dorsal side all the way to the tail. The incision needs to be on your side of the back bones./7. Using the tip of the knife, extend the incision towards the belly along the backbones. It is easier if you lift the flesh that is already removed from the bones so that you can see where your knife is cutting./8. Detach the rib cage by cutting the rib bones along the back bones./9. Continue to remove the flesh along the back bones until you reach to the belly, but keep the belly skin intact. You now have a butterflied fish with the bone in./10. Flip the butterflied fish over (skin side up) and make an incision on the other side of the dorsal in the same way./11. Chop the backbone at the tail end, keeping the tail attached to the flesh./12. Now you have a butterflied fish fillet. If small pieces of guts are left on the belly, wipe them off using kitchen paper./13. Place the tip of the knife where the rib bones start and trim the flesh with the rib bones very thinly. Do the same on the other side of the rib bones./14. There is a very sharp hard thorn in front of the anal fin. You need to remove it. I used kitchen scissors for this./15. The last step is to remove the pin bones from the fillet. Run your finger along where the backbone was and feel the bones to locate them. Remove all of them using a pair of fish bone tweezers or pliers./16. Sprinkle salt and pepper over both sides of butterflied fish fillets./17. Working one fillet at a time, coat a fillet with flour, then pat to shake off excess flour. Place it in the egg and coat all over. Allow excess egg to drip, then transfer to the breadcrumbs./18. Cover the entire fish with breadcrumbs, and gently press down so that a good layer of breadcrumbs is stuck on both sides. Repeat for the rest of the fillets./19. Heat oil in a frying pan to 170 degrees C / 338 degrees F. The oil should be about 3cm / 1.25" deep./20. Gently place the crumbed fish skin side up. Do not crowd the oil with too many fish pieces. Cook for about 1-1.5 minutes, then turn the fish over. Cook for further 1 minutes or so, until golden brown./21. Transfer the fried fish to a tray lined with kitchen paper to drain excess oil./22. Place two Aji Fry pieces with shredded lettuce on each serving plate. Serve immediately with the sauce of your choice. </t>
-  </si>
-  <si>
     <t>1*package*Nissin Chicken Ramen,400*ml*Boiling Water,1*slice*Cooked Ham,0.5*null*Hard Boiled Egg,0*null*Chopped Green Onion</t>
   </si>
   <si>
@@ -359,7 +299,67 @@
     <t xml:space="preserve">53*grams*Vegetable Oil, 3*null*Eggs, 90*mL*Water, 1*tablespoon*Vanilla Extract, 140*grams*Cake Flour, 268*grams*Granulated White Sugar, 0.5*tablespoon*Baking Powder, 0.25*teaspoon*Salt, 0.5*teaspoon*Cream of Tartar, 90*grams*Egg Whites (Room temp), 225*grams*Unsalted Butter (Room temp &amp; cubed), 0.5*teaspoon*lemon juice, 1*teaspoon*Lemon Zest, 0*null*Yellow Food Colouring </t>
   </si>
   <si>
-    <t xml:space="preserve">1. Heat up the oil and add the onions. Cook in med low until they are slightly soft and slightly see through not all the way. about 3-5 mins./2. Add the garlic and cook on low for another 3 minuets till everything is soft and slightly colored. Don't cook it till it’s brown then it’ll be burnt and wont taste good./3. Open the can of crushed tomatoes and add it. Cook on med low for about 10 mins./4. Add the bay leafs, Italian spices, salt, and pepper and if you have some fresh basil stir everything and let it cook for another 10-15 minuets. Now if you arent sure about how much spices you want I would add a little bit and add more if you feel like you need it. It is easier to add then to take away and you dont want the sauce to be ruined by over seasoning it./5. After the sauces has been cooking I like to taste it at this point and see how it tastes. Then I’ll add the sugar again same thing add a little and taste till it’s perfect for you. I then cook for another 5 minutes and then turn the heat off and let it stand./6. As the sauce is standing I start the pasta. Just put a pot of water on the stove and wait for it to boil.Once it’s boiling I add a little salt and oil this keeps the pasta from sticking and gives it a little bit of a taste./7. I like my pasta al dente so I check after 9-10 minuets to see if it’s ready if you like it softer then wait longer./8. Strain the pasta heat up the sauce quickly if it’s cooled too much and it’s done!/9. </t>
+    <t xml:space="preserve">1.Heat 2 tbsp oil in pan, add mushroom and saute till fragrant.||2. Add in bamboo shoots and pork fillet. Fry till meat turn white.||3. Add in seasoning and fried shallots and mix evenly. Remove from heat and set aside.||4. Combine flour with water in a small mixing bowl, stir till well dissolved.||5. Bring a pot of water to a simmer. Place the bowl of flour batter over the pot. Stirring constantly and cook till batter turns thick.||6. Grease 4 small bowls with corn oil. Scoop some cooked batter into each bowl. Lightly grease your fingers and press out the dough to cover the base of the bowl. Fill in meat filling. Top with another layer of cooked dough covering the fillings completely. Using greased fingers to smoothen out the edge and surface. ||7. Steam the meatballs over preheated steamer over high heat for 10 minutes. Cool down for 10 minutes.||8. Heat some oil in pan, remove the meatballs from the bowl and pan fry them till lightly brown on both sides. Drain well and serve with sauce immediately.||9. Optional sauce: mix and simmer 2 tablespoons sweet chilli sauce, 1 tablespoon miso paste, 4 tablespoon Hai Shan sauce, 1 tablespoon sugar, 100mL water. Add in corn starch after simmering to thicken. </t>
+  </si>
+  <si>
+    <t>1. Boil the water.||2. Place the noodles in a ramen bowl. Pour boiling water over the noodles and cover. Set and start your timer for three minutes.||3. After the first minute, quickly open, shake the noodles to separate, then arrange the ham, egg, and green onion over the noodles. Cover again and wait until the timer beeps.</t>
+  </si>
+  <si>
+    <t>1. In a medium bowl, whisk the salt into the flour. In a large mixing bowl on med-high speed, cream together the butter &amp; sugar until light &amp; fluffy. Mix in the egg &amp; flavoring until fully combined. Turn the speed to low &amp; gradually add in the flour &amp; beat until a smooth dough is formed. Lay out a large sheet of plastic wrap &amp; plop the cookie dough into the center. Wrap the dough &amp; shape it into a log about 1.5 inches in diameter. Wrap it again is foil &amp; then place it in the fridge for a couple hours or overnight.||2. Line 2 large trays with parchment. Remove the dough from the fridge &amp; cut it into even slices between 0.25 inches - 0.5 inches wide (this will give you uniform cookies). Roll 1 slice at a time in the palms of your hands to make dough balls &amp; place them on the trays about 2 inches apart. Press your thumb into the center of each ball to make a decent indentation, being careful not to go all the way through to the tray below (also, having short thumb nails is best). If the sides crack, simply press them back together.||3. If you're using fruit preserves for the center, spoon a small amount into each thumbprint. Do not mound up the preserves, just let it be a flat little pool. If you're using candied cherries, simply cut them in half &amp; nestle one half-round side up-into each thumbprint. If using maraschino cherries, do the same thing after you've drained &amp; patted||gently squeezed them dry.||4. Chill the cookie trays in the fridge while your oven preheats to 350degreesF. Bake 1 tray at a time on the middle rack for about 12 minutes, or until the cookie bottoms are just beginning to golden. Remove from the oven &amp; gently transfer the cookies to a cooling rack. If you'd like to sprinkle sugar over the cookies (gives them a more Christmas-y vibe), place the cooling rack over the empty baking tray &amp; dust the cookies with sifted powdered sugar, &amp; then let cool. To store, place in an airtight container with wax paper.</t>
+  </si>
+  <si>
+    <t>1. Fry strips of bacon in a cast iron skillet over medium low heat. This keeps the bacon from burning while the fat renders out.|| 2.Once the fat has rendered out, add cracked eggs to the pan. Cook until the eggs have a good crust on them. If the whites need to cook more, kill the heat to the pan and cover with a lid to steam the tops of the egg whites.||3. Serve the eggs and bacon with some sliced bread and cheese and a good sprinkle of salt and pepper. Enjoy!</t>
+  </si>
+  <si>
+    <t>1. Cut up the potatoes and put them in a pot of boiling water.  Boil for about 5 minutes, then add in two eggs and boil for 5 more minutes.  Take out the eggs, and strain the potatoes.  Then mash the potatoes in a bowl with 0.6 cup of milk.||2.Add the mashed potatoes to the bottom of your casserole dish, saving about 1 potato worth of mash in the bowl.||3. Slice all of the vegetables and the hardboiled eggs and saute them in a pan with some oil or butter and the bay leaves.||4. Add in the rest of the milk, the mashed potato that you saved, mustard, salt and pepper.  Cook everything on medium heat stirring occasionally, until the milk reaches a thick consistency, then add it into the casserole pan.  Remember to remove the bay leaves.||5. Cut the fish fillets into 3 inch wide chunks, and then add it into the casserole pan.||6. Unroll the pie crust and put it on top. You can cut it into strips, and cut out a fish if you want to make it like the one in Kiki's Delivery Service. Once you finish covering the casserole pan with the pie crust, beat an egg and brush it on top of the pie crust.||7. Bake in a 350 degree oven for about 20-30 minutes, or until the crust is to your liking.</t>
+  </si>
+  <si>
+    <t>1. You'll actually want to start with your frosting, since it needs extra time to chill (in fact, you can make the frosting a day ahead of time if you want). First, place your chocolate chips in a large bowl and set aside.||2. Cook the whipping cream and butter in a saucepan over medium heat until just boiling, stirring frequently. Pour the cream mix over the chocolate and whisk briskly until completely smooth.||3. Place some plastic wrap over the bowl and put it in the fridge to chill. After 1 hour, stir the mix thoroughly. Replace the cover and put the mix back in the fridge for another hour or until it reaches spreading consistency.||4. While you're waiting for the frosting to chill, you can bake your cake! Preheat your oven to 350 degrees. Thoroughly spray a 9-inch round cake pan with cooking spray or grease it with butter and flour. This cake likes to stick, so be sure to thoroughly coat every nook and cranny.||5. Dump the sugar, flour, cocoa, baking soda, baking powder, and salt into a large bowl. Whisk it all up!||6. Whisk in the egg, buttermilk, coffee, oil and vanilla. Beat the mix briskly for 2 minutes.||7. Pour the batter into your pan and bake for 25-30 minutes or until a toothpick inserted in the center comes out clean.||8. When fully baked, set the cake pan on a wire rack to cool for 10 minutes. Then flip the cake out of the pan and allow it to cool completely on the rack.||9. When the cake is cool, spread on a layer of chocolate frosting. Let it set for 5-10 minutes.||10. Use a toothpick to draw out where you'll put the decorative icing. This makes it easier to replicate the look of the cake in the movie. If you make a mistake, just use an icing knife or butter knife to smooth it out.||11. Pipe your decorative icing over the toothpick drawing and allow it to set for another 5-10 minutes.</t>
+  </si>
+  <si>
+    <t>1. Cook Rice.||2. Prepare Shishamo fish: Shishamo fish (or like fish) is usually sold frozen. Defrost and set frying pan to medium heat. And some oil and cook shishamo for about 5 minutes until crispy. Flip over and cook the other side for another 5 minutes. Place on a paper towel to soak the extra oil.||3. Prepare the Sakura Denbu: Sakura Denbu is a type of furikake, a condiment to put on top of rice. It's salty-sweet and commonly pink to represent cherry blossoms. Boil water and add kombu and whole cod. The cod is cooked when you can break it into pieces easily. Drain the cod well. Use a paper towel to squeeze out the extra water from the fish. The dryer, the better is will look as flakes. On a plate, take out any extra bones. Prepare a pan or pot on medium-low heat. Add 2 Tbsp sake, 2 Tbsp sugar, 1 tsp salt to pan, then add the cod. Use chopsticks or other utensil that will break the cod into small flakes. Stir well until liquid evaporates. Lower the heat if the cod starts to over cook. Remove from heat once liquid evaporates. Add two drops of red food coloring and add a little bit of water (you can make the color light or darker to your choosing). Add the food coloring mixture to the cod.  Put under low heat if the flakes get mushy from the water.  Mix well until you get your desired pink color.||4. Prepare the edamame: Boil frozen edamame for 6-10 minutes. Drain water in a colander and shuck the beans.||5. Assemble all in the lunch box to look cute.</t>
+  </si>
+  <si>
+    <t>1. Preheat your oven to 150C. In a small saucepan add in your butter and milk and over medium heat, melt the butter, stirring occasionally. Remove from heat to slightly cool before using. Optional: You can also melt down 1 tbsp of honey with this mixture if you don't like eggy tasting cakes.||2. Separate the whites and yolks of the eggs. Leave whites aside for meringue.||3. Sieve the flour into a large mixing bowl. Add in your warm butter and milk mixture until well combined (it may look like dough, that's okay). Then in 3-4 additions, mix in your egg yolks until you have a thick batter. Optional: Add 1 tsp of vanilla extract with eggs if you don't like eggy tasting cakes.||4. Whisk your egg whites on medium speed while adding your sugar in a slow, steady stream. Once all the sugar is added, continue whisking until you reach soft peaks (mixture will stay on your whisk, but the tip of the meringue droops).||5. Add your egg yolk mixture to the meringue and gently fold the two mixtures together until well combined and homogenous in colour.||6. Line your baking tins with non-stick spray and baking paper, ensuring to leave overhang for easy removal. Wrap the base of the cake tins with aluminum foil (if they're loose bottom) to ensure water doesn't get into the cakes.||7. Divide the batter between the two tins, and level out the surfaces. Place on your baking||roasting tray and fill with 2cm worth of hot water.||8. Transfer into oven and bake at 150c for 1 hour and the cakes are golden brown.||9. Remove cakes from the oven and allow to cool for 10 minutes before removing from tins to fully cool.||10. In a medium saucepan, bring the water to a boil and stir in gelatin or agar until fully dissolved. Mix in red bean paste until dissolved, thick and glossy. Set aside to cool.||11. Line one baking tin with plastic wrap on all sides, ensuring to leave overhang for easy removal. Place 1 cake, golden side down into the tin. Then add the red bean paste, spreading it out in an even layer. Then, top with remaining cake, golden side up. Refrigerate for 4 hours or until red bean filling is set.||12. When the filling is set, remove the cake from the tray, trim the edges of the cake to show off the well-defined layers. Cut the cake into 8 equal triangles and enjoy!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Heat up the oil and add the onions. Cook in med low until they are slightly soft and slightly see through not all the way. about 3-5 mins.||2. Add the garlic and cook on low for another 3 minuets till everything is soft and slightly colored. Don't cook it till it’s brown then it’ll be burnt and wont taste good.||3. Open the can of crushed tomatoes and add it. Cook on med low for about 10 mins.||4. Add the bay leafs, Italian spices, salt, and pepper and if you have some fresh basil stir everything and let it cook for another 10-15 minuets. Now if you arent sure about how much spices you want I would add a little bit and add more if you feel like you need it. It is easier to add then to take away and you dont want the sauce to be ruined by over seasoning it.||5. After the sauces has been cooking I like to taste it at this point and see how it tastes. Then I’ll add the sugar again same thing add a little and taste till it’s perfect for you. I then cook for another 5 minutes and then turn the heat off and let it stand.||6. As the sauce is standing I start the pasta. Just put a pot of water on the stove and wait for it to boil.Once it’s boiling I add a little salt and oil this keeps the pasta from sticking and gives it a little bit of a taste.||7. I like my pasta al dente so I check after 9-10 minuets to see if it’s ready if you like it softer then wait longer.||8. Strain the pasta heat up the sauce quickly if it’s cooled too much and it’s done!||9. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Gather all the ingredients. I follow a rice-to-water ratio of 1 to 5 for a thicker consistency in this recipe; to adjust for a runnier consistency, please see the Notes at the end of the recipe card.||2. Rinse 0.25 cup uncooked Japanese short-grain white rice in water, then drain. Repeat until the water runs clear. Drain into a colander and shake off the excess water.||3. Add the well-drained rice and 250 ml water to a heavy-bottomed pot or a donabe earthenware pot, as I have here. If cooking in a donabe, use a towel to wipe off any excess water on the bottom of the pot (or else it may crack under heat). Tip: Select a cooking pot with plenty of room for the rice and water to cook without boiling over.||4. Soak the rice for at least 30 minutes.||5. Cover the pot and bring to a boil over high heat.||5. Once boiling, lower the heat to the stove's lowest setting (make sure to use the right size of stove burner for your pot size). Open the lid and gently mix with a spoon, making sure the rice does not stick to the bottom of the pot.||6. Then, cover with the lid and gently simmer the rice for 30 minutes. During this time, I do not open the lid or mix the rice. Tip: With a good size pot and the lowest heat on the stove, the water should not boil over. If you cook with more water or your pot is smaller than mine, you may want to leave the lid slightly ajar so the water doesn't boil over. Tip: If you are worried, you can take a quick peek to make sure there's enough water so the rice doesn't burn on the bottom of the pot. If necessary, you can stir the rice or add a bit of hot water. Otherwise, don't stir the rice because that may break the rice grains.||7. After 30 minutes, turn off the heat and let it steam with the lid on for 10 minutes. The rice porridge should be soft and thick. If you want to add a beaten egg or salt, this is the time to mix it in. I keep this recipe plain and simple. Serve in individual rice bowls and garnish with toppings of your choice.||8. You can keep the leftovers in an airtight container and keep them for 2 days in the refrigerator or for up to a month in the freezer. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Add the flour, sugar, yeast and salt into a bowl, ensuring that the salt and yeast aren't touching. Mix thoroughly to combine. Add the water and oil, then mix with a wooden spoon until it comes together as a rough dough.||2. Turn the dough out onto a lightly floured work surface and knead by hand (or in a stand mixer) for 10 minutes or until soft, smooth and elastic.||3. Lightly coat a bowl in oil and transfer in your dough. Toss the dough in the bowl to ensure it's fully coated in oil. Cover and allow to proof until doubled in size (about an hour).||4. Uncover the dough and knock out the air. Flatten the dough into a large disc and make a well in the centre. Add the baking powder into the well and gather the edges of the dough towards the centre to enclose the baking powder.||5. Knead the dough for a few minutes or until the baking powder is well distributed into the dough. Flatten the dough and then divide the dough into 6 to 12 even pieces, cover any dough that isn't being used to prevent it from drying out.||6. Pat out your portioned dough into a disc and spread over a layer of red bean paste. Cup the dough in both hands and gently rotate the dough until the edges are nearly touching. Gather the edges together and twist to seal. Invert the dough so that the seam is on your work surface. Gently roll it around to help tighten that seal. Cover and rest the buns for another 20 minutes. Line your steamers and bring water to a boil in a saucepan during that time.||7. Transfer the buns into a steamer lined with some baking paper, making sure to leave space between each bun as they will expand. Cover with a lid, place the steamer onto your saucepan, reduce heat to a simmer and allow to steam, undisturbed for 12 to 15 minutes (20 minutes if you want to make a massive one). Remove from heat and allow to rest for 5 minutes before opening the lid. Eat them while they're still warm! </t>
+  </si>
+  <si>
+    <t>1. Start by slicing your nori sheets in half lengthwise. My sheets were 2.5 inches x 3.5 inches, so in the end I had 12 strips that were 1.25 inches wide. Mix the mayonnaise into your salmon until well coated. Set the salmon mix and nori aside.||2. Put the cookie cutter on a flat surface. Place an 8x8 inches sheet of plastic wrap over the cookie cutter and push some of it it down inside so that the inside of the cookie cutter is completely lined with plastic wrap. Scoop approximately 2 tbsp of rice into the bottom of the cutter and press it flat with a plastic spoon or small rubber spatula (the rice won't stick to the tools as much as it sticks to fingers!). When flattening the rice, push it around so that it reaches right up to the corners of the cutter (add more rice if needed to make sure the bottom is completely coated). Place 1 tsp salmon filling into the middle of the rice, spreading it around just a little, so there will be a little salmon in each bite of rice when you're finished.||3. Place a couple more tablespoons of rice on top and flatten out as before. Add a little extra rice if you need more to cover up the salmon. Wrap the plastic tightly over the exposed end of the onigiri and pop it out of the cookie cutter. Firmly wrap any loose ends around the outside of the onigiri. Set aside. ||4. Repeat with remaining rice and salmon until you run out of ingredients (for me, this made 12 rice balls).||5. Let the onigiri set for 5-10 minutes. If planning to eat them later, place them on a baking sheet and chill until ready to serve (you can reheat them in the microwave inside the plastic wrap for no more than 20-25 seconds - if they get too hot, they can fall apart). ||6. When ready to serve, remove the plastic wrap and press a nori strip around the bottom of each onigiri. The rice should still be sticky enough that the nori adheres with no problems.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Preheat oven to 160C fan forced.||2. In the bowl of a stand mixer, add the oil, egg yolks, water and vanilla extract. Beat over medium-high speed for 30 seconds or until emulsified.||3. Sift in the flour, baking powder, salt and add 118 grams of white sugar. Beat over medium speed until just combined and no lumps remain, about 1-2 minutes.||4. In a separate bowl, whisk the egg whites (NOT the 90g Egg whites) until foamy. Add the cream of tartar and continue whisking until soft peaks are achieved.||5. Then slowly add in 50 grams of white sugar and continue to whisk until the meringue reaches stiff peaks.||6. Add a third of the meringue into the egg-yolk batter and whisk to combine. Add another third of the meringue and gently fold together until no white streaks remain. Repeat folding process with the final a third of the meringue.||7. Line the base of a loose bottomed 8-inch cake pan with oil and baking paper. Gently pour the mixture into the pan, smooth the surface with a spatula and tap against the counter a few times to level the cake.||8. Transfer into the oven and bake for 45-50 minutes, or until a skewer can be inserted into the centre of the cake and when removed, it comes out clean. Allow to cool completely in the pan.||9. Over a pot of simmering water, place over a stand mixer||heatproof bowl ensuring the water is not touching the bowl.||10. Add 100g sugar, egg whites, lemon juice and lemon zest into the bowl and whisk until sugar is completely dissolved.||11. Remove the bowl and attach to your stand mixer. Whisk meringue over high speed until the meringue and bowl are cool to the touch.||12. Reduce speed to medium-low and add in the softened butter 1tbsp at a time, ensuring each addition of butter is fully incorporated before adding more. Scrape down the bowl as necessary.||13. After adding all the butter, beat for an additional 2 minutes.||14. To ice the cake, apply a thin layer of buttercream all over the cake and refrigerate for 10-15 minutes or until the buttercream is firm to the touch. Once firm, remove from the fridge and apply a final layer of buttercream onto the cake. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. In a large bowl, beat the butter until light and creamy.||2. Add the sugar and beat together until well combined.||3. Add the vanilla and salt, continue to beat while adding the beaten egg in 3 to 4 additions.||4. Add the flour and knead together until a cohesive dough is formed.||5. Reserve half the dough to one side, adding the cocoa powder to the other half. Knead until well combined.||6. Place each dough onto a sheet of baking paper. Pat into a flat rectangle, top with another sheet of baking paper and roll until 5mm in thickness. Refrigerate for 1 hour or until firm.Preheat oven to 160C fan forced.||7. Cut the vanilla cookies into squares, then score horizontal and two vertical lines perpendicular to the edges of the cookies. Transfer to a lined baking tray.||8. Cut the chocolate cookies using a 48mm fluted cookie cutter. Transfer to a lined baking tray, then cut out the centre of each cookie with a small round cutter||piping tip.||9. Bake both sheets of cookies for 18-20 minutes. Remove chocolate cookies after 12 minutes, add in 0.5 tsp of crushed candy to each cookie centre, then continue to bake for remaining time.||10. Allow to cool on the tray for 10 minutes before transferring to a wire rack. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Remove the scales on both sides of the fish by sliding the tip of the knife from the tail end towards the head.||2. Place the knife where the tail begins, facing the blade to the head. Move the knife at a very low angle towards the head and trim the bony scales (scutes) along the lateral line, which ends close to half-way.||3. Remove the head by cutting at a slight angle behind the gill and the front fin.||4. Using a finger or a narrow knife, remove the guts from the opening, without breaking the thin flesh around the belly.||5. Rinse the fish and clean the cavity in the belly. Pat dry, including inside the cavity. ||6. Starting from the head of the fish, make a shallow incision on the dorsal side all the way to the tail. The incision needs to be on your side of the back bones.||7. Using the tip of the knife, extend the incision towards the belly along the backbones. It is easier if you lift the flesh that is already removed from the bones so that you can see where your knife is cutting.||8. Detach the rib cage by cutting the rib bones along the back bones.||9. Continue to remove the flesh along the back bones until you reach to the belly, but keep the belly skin intact. You now have a butterflied fish with the bone in.||10. Flip the butterflied fish over (skin side up) and make an incision on the other side of the dorsal in the same way.||11. Chop the backbone at the tail end, keeping the tail attached to the flesh.||12. Now you have a butterflied fish fillet. If small pieces of guts are left on the belly, wipe them off using kitchen paper.||13. Place the tip of the knife where the rib bones start and trim the flesh with the rib bones very thinly. Do the same on the other side of the rib bones.||14. There is a very sharp hard thorn in front of the anal fin. You need to remove it. I used kitchen scissors for this.||15. The last step is to remove the pin bones from the fillet. Run your finger along where the backbone was and feel the bones to locate them. Remove all of them using a pair of fish bone tweezers or pliers.||16. Sprinkle salt and pepper over both sides of butterflied fish fillets.||17. Working one fillet at a time, coat a fillet with flour, then pat to shake off excess flour. Place it in the egg and coat all over. Allow excess egg to drip, then transfer to the breadcrumbs.||18. Cover the entire fish with breadcrumbs, and gently press down so that a good layer of breadcrumbs is stuck on both sides. Repeat for the rest of the fillets.||19. Heat oil in a frying pan to 170 degrees C || 338 degrees F. The oil should be about 3cm || 1.25 inches deep.||20. Gently place the crumbed fish skin side up. Do not crowd the oil with too many fish pieces. Cook for about 1-1.5 minutes, then turn the fish over. Cook for further 1 minutes or so, until golden brown.||21. Transfer the fried fish to a tray lined with kitchen paper to drain excess oil.||22. Place two Aji Fry pieces with shredded lettuce on each serving plate. Serve immediately with the sauce of your choice. </t>
+  </si>
+  <si>
+    <t>1. Cut the spinach into 5 cm width.||2. Put oil in a frying pan and fry the spinach.||3. Season with salt, add sesame seeds and mix.||4. Crack 2 eggs, add soy sauce and sugar, and mix.||5. Spread oil on a frying pan and spread 1||3 of the egg mixture. Fold the egg several times.||6. Spread oil again, add half of the remaining egg mixture and spread. Fold the eggs together with (5).||7. Spread the oil again, add the rest of the egg mixture, spread it out, and fold the egg of (6).||8. Add the seasoning for the bonito flakes to the frying pan, mix, and bring to a boil.||9. Add katsuobushi and mix.||10. Lightly heat the mentaiko.||11. Cut the mentaiko in half and the egg into bite-sized pieces.||12. Arrange in a bento box with rice, ham, and natto.||13. Serve with miso soup on the side</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Cut the carrots evenly: put your peeled carrot on the board, and cut at even intervals while giving a quarter-turn to the carrot each time. Or alternatively, slice carrots regularly and use a cookie cutter to create flower shaped carrots.||2. Cut and prep the potatoes into fairly even pieces. Optionally, you can shave the edges of each piece to round them off. This cutting method is called mentori. Put the cut up potato in a bowl of water, and then drain to rinse off the surface starch||3. Cut the shiitake mushtooms: tightly squeeze out the rehydrated dried shiitake mushrooms, saving the soaking liquid. Cut off the stem, which is usually too chewy even after rehydrating. Cut each cap in half - but instead of just going straight up and down, make a slanted 45 degree cut.||4. Cut the onion into one 8th wedges.||5. Heat up your pan with the teaspoon of oil.  Put the onions in first and stir around for 2-3 minutes until the edges start turning a bit translucent.||5. Add the potatoes and carrots and continue stirring for a minute. This short sauteing step helps to bring out the sweetness of the vegetables. Add the mushrooms and stir a bit more.||6. Add the dashi stock (or combined dashi + mushroom soaking liquid). There should be enough to just about come to the top level of all the vegetables in the pot.||7. Bring it up to a boil and lower the heat to a simmer. Some scum will rise to the top, which should be removed so that the final dish will have a clean taste and appearance. Try to take off just the scum and leave the liquid. ||8. Add the flavoring ingredients in this order: sugar, mirin, sake, and then finally the soy sauce.||9. Let simmer on its own. In the meantime, blanch the peas in boiling water for a minute or two.||10. Arrange the vegetables attractively in a bowl, pouring a little of the cooking liquid over it to add shine and flavor. Garnish with the snow peas or other green garnish of your choice to make it pop. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. In a large measuring cup or bowl, combine 3.3 cups dashi (Japanese soup stock), 2 Tbsp mirin, 2 Tbsp soy sauce, and 1 tsp Diamond Crystal kosher salt.||2. Mix it all together until the salt is completely dissolved. Then, divide the soup broth into the individual donabe clay pots. Set aside.||3. Cut 1 inch kamaboko (fish cake) into 4 thin slices about 0.25 inch thick. Cut 1 piece aburaage (deep-fried tofu pouch) into 4 rectangular pieces.||4. Cut off and discard the stems of 2 shiitake mushrooms.||5. Slice 1 Tokyo negi (naga negi; long green onion) diagonally into 0.5-inch (1.3-cm) pieces.||6. Cut 2 stalks komatsuna or other green vegetable into 2-inch (5-cm) pieces. Keep the stem and leafy parts separate because we will add them to the broth at different times.||7. To cook 2 servings udon noodles, bring a large pot of water to a boil. Once boiling, cook the frozen udon for 1 minute until heated through and drain well. If you use dried noodles, cook them according to the package instructions.||8. Divide and add the udon noodles into the individual pots. Then, top the noodles with equal portions of the kamaboko fish cake, aburaage, shiitake mushroom, Tokyo negi, and green vegetable stems. (Set aside the eggs, leafy greens, and shrimp tempura for later.)||9. Transfer the pots to individual burners on the stovetop. Cover with the lids and bring the soup to a boil over medium heat. Once boiling, reduce the heat to a simmer and cook for 2-3 minutes.||10. Uncover the pot. With 2 large eggs (50 g each w||o shell), crack one egg in the center of each pot on top of the ingredients. Cover to cook until the egg is done to your liking.||11. Once the egg is done, add both the leafy greens and the cooked 4 shrimp tempura on top.||12. Bring the donabe to the table. Sprinkle with shichimi togarashi (Japanese seven spice) and top with yuzu zest, if you'd like. </t>
+  </si>
+  <si>
+    <t>1. Prepare a bowl of rice.||2. Crack the egg on top of the rice.||3. Drizzle with soy sauce to taste.||4. Mix well.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Remove salmon skin and season the salmon with salt and pepper.||2. Add 2 tbsp of butter into a saucepan and heat on medium-low. Fry the salmon until both sides turn golden brown.||3. Melt 2 tbsp of butter in a saucepan over medium heat. Add chopped garlic and shallots. Stir well until the garlic turns light brown.||4. Lower the heat to medium-low and add flour. Mix well until the mixture thickens.||5. Add milk while stirring. Mix until the mixture thickens again.||6. Add baby carrots and 1 cup of water until it boils. Poke the carrots with a fork to check if it is soft enough.||7. Drain the baby carrots and add 2 tbsp of butter. Add salt and pepper as seasoning.||8. Add 2 tbsp of brown sugar. Mix well until the mixture thickens.||9. Transfer the salmon onto a plate and pour the cream sauce over it. Place the glazed carrots on the side of the plate. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Chop the carrots, broccoli, cauliflower, and potatoes into small pieces.||2. Slice the leek into thin slices.||3. Mince the garlic.||4. Heat olive oil on medium heat and cook the sliced leeks till it has softened.||5. Add about 5 cups of water and 1 tsp of salt.||6. When the water has reached a boil, add all of the chopped vegetables. Make sure that the vegetables are fully submerged in water.||7. Boil for less than 5 minutes. Pierce with a fork to see if the vegetables are soft enough.||8. Remove the vegetables from the pot and set it aside. ||9. With the remaining water left in the pot, add flour and milk. Whisk until it reaches a thick consistency.||10. Boil the mixture while whisking. Add the boiled vegetables and season it with salt and pepper.||11. Transfer it to a bowl and garnish with parsley. </t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -427,9 +427,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -768,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D3E378D-9781-4302-9477-07B2B463A36A}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D9" zoomScale="92" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -816,476 +813,476 @@
         <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="F2" s="1">
         <v>3</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="319" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="F3" s="1">
         <v>720</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="F4" s="1">
         <v>5</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="203" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="F5" s="1">
         <v>40</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F6" s="1">
         <v>150</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="D7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="F7" s="1">
         <v>30</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="362.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="E8" s="3" t="s">
-        <v>36</v>
+        <v>94</v>
       </c>
       <c r="F8" s="1">
         <v>720</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="232" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>107</v>
+        <v>85</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="F9" s="1">
         <v>40</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="333.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F10" s="1">
         <v>65</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="203" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="F11" s="1">
         <v>40</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="304.5" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="319" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="F12" s="1">
         <v>120</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F13" s="1">
         <v>15</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="348" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="F14" s="1">
         <v>150</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="203" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F15" s="1">
         <v>150</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F16" s="1">
         <v>50</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="D17" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="F17" s="1">
         <v>15</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="319" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F18" s="1">
         <v>40</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F19" s="1">
         <v>30</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="F20" s="1">
         <v>2</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="145" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="F21" s="1">
         <v>20</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="F22" s="1">
         <v>30</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Changing special ' to correct '
</commit_message>
<xml_diff>
--- a/database/COSC345_Recipes (1).xlsx
+++ b/database/COSC345_Recipes (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadia\Downloads\UNI-work\COSC345\Realm-of-Feasts\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B27A680-6F61-4242-A969-1AA988DEA456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1124E781-1284-4822-B267-8ED8402B68A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{D48BFF6E-7DE3-47B5-ADE0-6EAA34E0C134}"/>
   </bookViews>
@@ -323,9 +323,6 @@
     <t>1. Preheat your oven to 150C. In a small saucepan add in your butter and milk and over medium heat, melt the butter, stirring occasionally. Remove from heat to slightly cool before using. Optional: You can also melt down 1 tbsp of honey with this mixture if you don't like eggy tasting cakes.||2. Separate the whites and yolks of the eggs. Leave whites aside for meringue.||3. Sieve the flour into a large mixing bowl. Add in your warm butter and milk mixture until well combined (it may look like dough, that's okay). Then in 3-4 additions, mix in your egg yolks until you have a thick batter. Optional: Add 1 tsp of vanilla extract with eggs if you don't like eggy tasting cakes.||4. Whisk your egg whites on medium speed while adding your sugar in a slow, steady stream. Once all the sugar is added, continue whisking until you reach soft peaks (mixture will stay on your whisk, but the tip of the meringue droops).||5. Add your egg yolk mixture to the meringue and gently fold the two mixtures together until well combined and homogenous in colour.||6. Line your baking tins with non-stick spray and baking paper, ensuring to leave overhang for easy removal. Wrap the base of the cake tins with aluminum foil (if they're loose bottom) to ensure water doesn't get into the cakes.||7. Divide the batter between the two tins, and level out the surfaces. Place on your baking||roasting tray and fill with 2cm worth of hot water.||8. Transfer into oven and bake at 150c for 1 hour and the cakes are golden brown.||9. Remove cakes from the oven and allow to cool for 10 minutes before removing from tins to fully cool.||10. In a medium saucepan, bring the water to a boil and stir in gelatin or agar until fully dissolved. Mix in red bean paste until dissolved, thick and glossy. Set aside to cool.||11. Line one baking tin with plastic wrap on all sides, ensuring to leave overhang for easy removal. Place 1 cake, golden side down into the tin. Then add the red bean paste, spreading it out in an even layer. Then, top with remaining cake, golden side up. Refrigerate for 4 hours or until red bean filling is set.||12. When the filling is set, remove the cake from the tray, trim the edges of the cake to show off the well-defined layers. Cut the cake into 8 equal triangles and enjoy!</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Heat up the oil and add the onions. Cook in med low until they are slightly soft and slightly see through not all the way. about 3-5 mins.||2. Add the garlic and cook on low for another 3 minuets till everything is soft and slightly colored. Don't cook it till it’s brown then it’ll be burnt and wont taste good.||3. Open the can of crushed tomatoes and add it. Cook on med low for about 10 mins.||4. Add the bay leafs, Italian spices, salt, and pepper and if you have some fresh basil stir everything and let it cook for another 10-15 minuets. Now if you arent sure about how much spices you want I would add a little bit and add more if you feel like you need it. It is easier to add then to take away and you dont want the sauce to be ruined by over seasoning it.||5. After the sauces has been cooking I like to taste it at this point and see how it tastes. Then I’ll add the sugar again same thing add a little and taste till it’s perfect for you. I then cook for another 5 minutes and then turn the heat off and let it stand.||6. As the sauce is standing I start the pasta. Just put a pot of water on the stove and wait for it to boil.Once it’s boiling I add a little salt and oil this keeps the pasta from sticking and gives it a little bit of a taste.||7. I like my pasta al dente so I check after 9-10 minuets to see if it’s ready if you like it softer then wait longer.||8. Strain the pasta heat up the sauce quickly if it’s cooled too much and it’s done!||9. </t>
-  </si>
-  <si>
     <t xml:space="preserve">1. Gather all the ingredients. I follow a rice-to-water ratio of 1 to 5 for a thicker consistency in this recipe; to adjust for a runnier consistency, please see the Notes at the end of the recipe card.||2. Rinse 0.25 cup uncooked Japanese short-grain white rice in water, then drain. Repeat until the water runs clear. Drain into a colander and shake off the excess water.||3. Add the well-drained rice and 250 ml water to a heavy-bottomed pot or a donabe earthenware pot, as I have here. If cooking in a donabe, use a towel to wipe off any excess water on the bottom of the pot (or else it may crack under heat). Tip: Select a cooking pot with plenty of room for the rice and water to cook without boiling over.||4. Soak the rice for at least 30 minutes.||5. Cover the pot and bring to a boil over high heat.||5. Once boiling, lower the heat to the stove's lowest setting (make sure to use the right size of stove burner for your pot size). Open the lid and gently mix with a spoon, making sure the rice does not stick to the bottom of the pot.||6. Then, cover with the lid and gently simmer the rice for 30 minutes. During this time, I do not open the lid or mix the rice. Tip: With a good size pot and the lowest heat on the stove, the water should not boil over. If you cook with more water or your pot is smaller than mine, you may want to leave the lid slightly ajar so the water doesn't boil over. Tip: If you are worried, you can take a quick peek to make sure there's enough water so the rice doesn't burn on the bottom of the pot. If necessary, you can stir the rice or add a bit of hot water. Otherwise, don't stir the rice because that may break the rice grains.||7. After 30 minutes, turn off the heat and let it steam with the lid on for 10 minutes. The rice porridge should be soft and thick. If you want to add a beaten egg or salt, this is the time to mix it in. I keep this recipe plain and simple. Serve in individual rice bowls and garnish with toppings of your choice.||8. You can keep the leftovers in an airtight container and keep them for 2 days in the refrigerator or for up to a month in the freezer. </t>
   </si>
   <si>
@@ -360,6 +357,9 @@
   </si>
   <si>
     <t xml:space="preserve">1. Chop the carrots, broccoli, cauliflower, and potatoes into small pieces.||2. Slice the leek into thin slices.||3. Mince the garlic.||4. Heat olive oil on medium heat and cook the sliced leeks till it has softened.||5. Add about 5 cups of water and 1 tsp of salt.||6. When the water has reached a boil, add all of the chopped vegetables. Make sure that the vegetables are fully submerged in water.||7. Boil for less than 5 minutes. Pierce with a fork to see if the vegetables are soft enough.||8. Remove the vegetables from the pot and set it aside. ||9. With the remaining water left in the pot, add flour and milk. Whisk until it reaches a thick consistency.||10. Boil the mixture while whisking. Add the boiled vegetables and season it with salt and pepper.||11. Transfer it to a bowl and garnish with parsley. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Heat up the oil and add the onions. Cook in med low until they are slightly soft and slightly see through not all the way. about 3-5 mins.||2. Add the garlic and cook on low for another 3 minuets till everything is soft and slightly colored. Don't cook it till it's brown then it'll be burnt and wont taste good.||3. Open the can of crushed tomatoes and add it. Cook on med low for about 10 mins.||4. Add the bay leafs, Italian spices, salt, and pepper and if you have some fresh basil stir everything and let it cook for another 10-15 minuets. Now if you arent sure about how much spices you want I would add a little bit and add more if you feel like you need it. It is easier to add then to take away and you dont want the sauce to be ruined by over seasoning it.||5. After the sauces has been cooking I like to taste it at this point and see how it tastes. Then I'll add the sugar again same thing add a little and taste till it's perfect for you. I then cook for another 5 minutes and then turn the heat off and let it stand.||6. As the sauce is standing I start the pasta. Just put a pot of water on the stove and wait for it to boil.Once it's boiling I add a little salt and oil this keeps the pasta from sticking and gives it a little bit of a taste.||7. I like my pasta al dente so I check after 9-10 minuets to see if it's ready if you like it softer then wait longer.||8. Strain the pasta heat up the sauce quickly if it's cooled too much and it's done!||9. </t>
   </si>
 </sst>
 </file>
@@ -765,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D3E378D-9781-4302-9477-07B2B463A36A}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="D9" zoomScale="92" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -940,7 +940,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="362.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="377" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -977,7 +977,7 @@
         <v>85</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="F9" s="1">
         <v>40</v>
@@ -986,7 +986,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="333.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="348" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>39</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F10" s="1">
         <v>65</v>
@@ -1046,7 +1046,7 @@
         <v>46</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F12" s="1">
         <v>120</v>
@@ -1069,7 +1069,7 @@
         <v>49</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F13" s="1">
         <v>15</v>
@@ -1078,7 +1078,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="348" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="362.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>50</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>86</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F14" s="1">
         <v>150</v>
@@ -1115,7 +1115,7 @@
         <v>54</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F15" s="1">
         <v>150</v>
@@ -1138,7 +1138,7 @@
         <v>58</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F16" s="1">
         <v>50</v>
@@ -1161,7 +1161,7 @@
         <v>62</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F17" s="1">
         <v>15</v>
@@ -1184,7 +1184,7 @@
         <v>66</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F18" s="1">
         <v>40</v>
@@ -1193,7 +1193,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="319" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>67</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>70</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F19" s="1">
         <v>30</v>
@@ -1230,7 +1230,7 @@
         <v>74</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F20" s="1">
         <v>2</v>
@@ -1253,7 +1253,7 @@
         <v>77</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F21" s="1">
         <v>20</v>
@@ -1262,7 +1262,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="145" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>78</v>
       </c>
@@ -1276,7 +1276,7 @@
         <v>81</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F22" s="1">
         <v>30</v>

</xml_diff>